<commit_message>
Loaded all ref EXCEL
Loaded all ref EXCEL
</commit_message>
<xml_diff>
--- a/CA/JIRA/PowerBI Input/THREE Component Development Locations cf v1-0 110320.xlsx
+++ b/CA/JIRA/PowerBI Input/THREE Component Development Locations cf v1-0 110320.xlsx
@@ -7,9 +7,7 @@
     <workbookView xWindow="0" yWindow="48" windowWidth="20100" windowHeight="9792"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Product_Components" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -810,28 +808,4 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Pie Chart and TreeMap
Added Pie Chart and TreeMap
</commit_message>
<xml_diff>
--- a/CA/JIRA/PowerBI Input/THREE Component Development Locations cf v1-0 110320.xlsx
+++ b/CA/JIRA/PowerBI Input/THREE Component Development Locations cf v1-0 110320.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="24">
   <si>
     <t>Component</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>Build Process</t>
+  </si>
+  <si>
+    <t>Workflow Configurator</t>
   </si>
 </sst>
 </file>
@@ -616,13 +619,12 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.88671875" customWidth="1"/>
+    <col min="1" max="2" width="20.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -793,10 +795,10 @@
     </row>
     <row r="16" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Updates to Dashboard One.
Updates to Dashboard One.
</commit_message>
<xml_diff>
--- a/CA/JIRA/PowerBI Input/THREE Component Development Locations cf v1-0 110320.xlsx
+++ b/CA/JIRA/PowerBI Input/THREE Component Development Locations cf v1-0 110320.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="24">
   <si>
     <t>Component</t>
   </si>
@@ -46,9 +46,6 @@
     <t>Watchlist Manager</t>
   </si>
   <si>
-    <t>Workflow Configuator</t>
-  </si>
-  <si>
     <t>Ireland</t>
   </si>
   <si>
@@ -86,13 +83,16 @@
   </si>
   <si>
     <t>Workflow Configurator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P&amp;C </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,6 +105,18 @@
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -182,7 +194,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -191,6 +203,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -316,7 +330,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C16" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C17" totalsRowShown="0" headerRowDxfId="3">
   <sortState ref="A2:C16">
     <sortCondition ref="A2:A16"/>
   </sortState>
@@ -616,10 +630,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -633,7 +647,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -647,7 +661,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -658,7 +672,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -669,62 +683,62 @@
         <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>10</v>
+        <v>15</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -735,7 +749,7 @@
         <v>6</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -746,7 +760,7 @@
         <v>5</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -757,51 +771,62 @@
         <v>4</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>14</v>
+      <c r="A13" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B16" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>23</v>
-      </c>
       <c r="C16" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>